<commit_message>
Updated login feature and admin inventory
</commit_message>
<xml_diff>
--- a/data/UserList.xlsx
+++ b/data/UserList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="442">
   <si>
     <t>Staff ID</t>
   </si>
@@ -1343,6 +1343,9 @@
   </si>
   <si>
     <t>Pwd129</t>
+  </si>
+  <si>
+    <t>Pwd122</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed logout/login bugs. Please HELP TO RETEST UR LOGIN/LOGOUT
</commit_message>
<xml_diff>
--- a/data/UserList.xlsx
+++ b/data/UserList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="477">
   <si>
     <t>Name</t>
   </si>
@@ -1445,6 +1445,12 @@
   </si>
   <si>
     <t>new@patient.com</t>
+  </si>
+  <si>
+    <t>new123</t>
+  </si>
+  <si>
+    <t>pendingU2</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1989,7 @@
         <v>23</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>336</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>24</v>
@@ -4999,7 +5005,7 @@
         <v>466</v>
       </c>
       <c r="G109" t="s" s="0">
-        <v>449</v>
+        <v>476</v>
       </c>
       <c r="H109" t="s" s="0">
         <v>465</v>
@@ -5086,7 +5092,7 @@
         <v>473</v>
       </c>
       <c r="G112" t="s" s="0">
-        <v>449</v>
+        <v>475</v>
       </c>
       <c r="H112" t="s" s="0">
         <v>474</v>

</xml_diff>